<commit_message>
nav bar has been added
</commit_message>
<xml_diff>
--- a/Tool.xlsx
+++ b/Tool.xlsx
@@ -2,18 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20354"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ecfile1.uwaterloo.ca\a25bharg\My Documents\MSCI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{957682AD-F29A-4C71-A4E0-096A8DA636E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97064D6C-0BBE-48EC-858B-DC9C41E3BE11}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7650" xr2:uid="{D9255281-5BC8-4E90-972C-CCC2897E7642}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" xr2:uid="{D9255281-5BC8-4E90-972C-CCC2897E7642}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Home" sheetId="1" r:id="rId1"/>
+    <sheet name="Contacts" sheetId="2" r:id="rId2"/>
+    <sheet name="Brainstorm" sheetId="3" r:id="rId3"/>
+    <sheet name="Software Library" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,16 +28,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="5">
   <si>
-    <t>test</t>
+    <t>Contact Book</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Brainstorm</t>
+  </si>
+  <si>
+    <t>Software Library</t>
+  </si>
+  <si>
+    <t>Contacts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -42,13 +57,61 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="22"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFF86A6A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFEDEDED"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEDEDED"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF86A6A"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -60,17 +123,45 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFEDEDED"/>
+      <color rgb="FFF86A6A"/>
+      <color rgb="FFE11F1F"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -379,20 +470,615 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EBC2B56-E393-4AC4-8110-6B9A294A9B6E}">
-  <dimension ref="A1"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:AR3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="K1" sqref="K1:P2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="12" max="12" width="9" customWidth="1"/>
+    <col min="27" max="143" width="0" hidden="1" customWidth="1"/>
+    <col min="150" max="725" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF1" s="3"/>
+      <c r="AG1" s="3"/>
+      <c r="AH1" s="3"/>
+      <c r="AI1" s="3"/>
+      <c r="AJ1" s="3"/>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="2"/>
+      <c r="AQ1" s="2"/>
+      <c r="AR1" s="2"/>
+    </row>
+    <row r="2" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="3"/>
+      <c r="AH2" s="3"/>
+      <c r="AI2" s="3"/>
+      <c r="AJ2" s="3"/>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="2"/>
+      <c r="AQ2" s="2"/>
+      <c r="AR2" s="2"/>
+    </row>
+    <row r="3" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="AE1:AJ2"/>
+    <mergeCell ref="K1:P2"/>
+    <mergeCell ref="H3:J3"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="H3:J3" location="Home!A1" display="Home" xr:uid="{E6B3F196-0C63-49BE-95DF-F3DF819A3103}"/>
+    <hyperlink ref="Q3:S3" location="'Software Library'!A1" display="Software Library" xr:uid="{DFA4BD81-6A97-4A53-9D31-8568D4FE8939}"/>
+    <hyperlink ref="N3:P3" location="Brainstorm!A1" display="Brainstorm" xr:uid="{8284AB99-903E-4EE7-AFF2-CAECBA2A9B4F}"/>
+    <hyperlink ref="K3:M3" location="Contacts!A1" display="Contact Book" xr:uid="{AF777A81-310B-4AE5-BC00-7070040242E3}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{443BD34C-7F79-463F-91DF-19684A1F6CE2}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:AR3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF1" s="3"/>
+      <c r="AG1" s="3"/>
+      <c r="AH1" s="3"/>
+      <c r="AI1" s="3"/>
+      <c r="AJ1" s="3"/>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="2"/>
+      <c r="AQ1" s="2"/>
+      <c r="AR1" s="2"/>
+    </row>
+    <row r="2" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="3"/>
+      <c r="AH2" s="3"/>
+      <c r="AI2" s="3"/>
+      <c r="AJ2" s="3"/>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="2"/>
+      <c r="AQ2" s="2"/>
+      <c r="AR2" s="2"/>
+    </row>
+    <row r="3" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="6" t="s">
         <v>0</v>
       </c>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="AE1:AJ2"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="K1:P2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="H3:J3" location="Home!A1" display="Home" xr:uid="{28D98482-0E63-4682-95CB-959F9F1137D6}"/>
+    <hyperlink ref="Q3:S3" location="'Software Library'!A1" display="Software Library" xr:uid="{3DD0AAA9-115B-414E-A9DF-A8E811B87F7C}"/>
+    <hyperlink ref="N3:P3" location="Brainstorm!A1" display="Brainstorm" xr:uid="{9ED983EB-7A16-4142-88A0-EB3894571A57}"/>
+    <hyperlink ref="K3:M3" location="Contacts!A1" display="Contact Book" xr:uid="{185F6CA2-4FFC-4ED3-8C2E-EC749FA3EAF2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57D7230D-C22E-4398-9DF8-725056486180}">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:AR3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF1" s="3"/>
+      <c r="AG1" s="3"/>
+      <c r="AH1" s="3"/>
+      <c r="AI1" s="3"/>
+      <c r="AJ1" s="3"/>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="2"/>
+      <c r="AQ1" s="2"/>
+      <c r="AR1" s="2"/>
+    </row>
+    <row r="2" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="3"/>
+      <c r="AH2" s="3"/>
+      <c r="AI2" s="3"/>
+      <c r="AJ2" s="3"/>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="2"/>
+      <c r="AQ2" s="2"/>
+      <c r="AR2" s="2"/>
+    </row>
+    <row r="3" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="AE1:AJ2"/>
+    <mergeCell ref="K1:P2"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="Q3:S3"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="H3:J3" location="Home!A1" display="Home" xr:uid="{A3B8396F-3BD4-4DFD-99E3-4E06C38C7718}"/>
+    <hyperlink ref="Q3:S3" location="'Software Library'!A1" display="Software Library" xr:uid="{76EC0A61-DBFE-44B6-99DA-5D52EA189DF2}"/>
+    <hyperlink ref="N3:P3" location="Brainstorm!A1" display="Brainstorm" xr:uid="{95EC4D9F-B2C7-497C-BC5C-6A5F2F7F9FBC}"/>
+    <hyperlink ref="K3:M3" location="Contacts!A1" display="Contact Book" xr:uid="{E487DF89-D115-4255-8791-453DA501C85E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9371A46-D7EB-443B-8AA7-1F594B82D174}">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:Z3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15:F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+    </row>
+    <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+    </row>
+    <row r="3" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="K1:P2"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="Q3:S3"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="H3:J3" location="Home!A1" display="Home" xr:uid="{1C0364A3-261B-42D1-AAE6-66C85DD9C709}"/>
+    <hyperlink ref="Q3:S3" location="'Software Library'!A1" display="Software Library" xr:uid="{13292B9C-2072-4FAB-85A9-84FEA8D46AF1}"/>
+    <hyperlink ref="N3:P3" location="Brainstorm!A1" display="Brainstorm" xr:uid="{F05A8EB7-54E6-4E73-A4D9-1CD305EF4273}"/>
+    <hyperlink ref="K3:M3" location="Contacts!A1" display="Contact Book" xr:uid="{B65DCAD9-7C24-459C-BDE7-CEE85F049685}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>